<commit_message>
6th july content added
</commit_message>
<xml_diff>
--- a/Assignmets/recordAssignments.xlsx
+++ b/Assignmets/recordAssignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\TeachingTraining\Assignmets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20E3A332-A460-4684-909A-5FC06B8F9C21}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0978808D-9D93-42C7-9633-93CB93827B21}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{5B3171BE-951C-4D0E-A378-BDA5E33214FC}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,9 +515,11 @@
       <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
       <c r="H3" s="2">
-        <f>SUM(B3:F3)</f>
+        <f>SUM(B3:G3)</f>
         <v>11</v>
       </c>
     </row>
@@ -540,9 +542,11 @@
       <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
       <c r="H4" s="2">
-        <f>SUM(B4:F4)</f>
+        <f>SUM(B4:G4)</f>
         <v>10</v>
       </c>
     </row>
@@ -565,9 +569,11 @@
       <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
       <c r="H5" s="2">
-        <f>SUM(B5:F5)</f>
+        <f>SUM(B5:G5)</f>
         <v>9</v>
       </c>
     </row>
@@ -590,9 +596,11 @@
       <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
       <c r="H6" s="2">
-        <f>SUM(B6:F6)</f>
+        <f>SUM(B6:G6)</f>
         <v>11</v>
       </c>
     </row>

</xml_diff>